<commit_message>
Move test case to Percentages section
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/NumberFormatTests.xlsx
+++ b/test-data/spreadsheet/NumberFormatTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyschott/repos/poi/test-data/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561825BC-2D13-D344-AE8C-042D33D20FE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD7B4B2-CA35-6F43-BBA5-C98D4633A221}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33140" windowHeight="22740" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="127">
   <si>
     <t>|?\:#=/=#|</t>
   </si>
@@ -466,16 +466,13 @@
   </si>
   <si>
     <t>#,##0.00%</t>
-  </si>
-  <si>
-    <t>Basic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -492,11 +489,6 @@
     <font>
       <sz val="10"/>
       <name val="Lucida Sans Typewriter"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -543,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -579,10 +571,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -993,9 +982,9 @@
   <dimension ref="A1:D337"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A286" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:XFD1"/>
-      <selection pane="bottomLeft" activeCell="A336" sqref="A336"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1232,31 +1221,31 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>0.04%</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="2">
-        <v>3.5E-4</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>127</v>
-      </c>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="9" t="str">
+        <f t="shared" ref="A17:A19" si="2">TEXT(C17, B17)</f>
+        <v>a $12.30 profit</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2">
+        <v>12.3</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="str">
-        <f t="shared" ref="A18:A20" si="2">TEXT(C18, B18)</f>
-        <v>a $12.30 profit</v>
+        <f t="shared" si="2"/>
+        <v>¥12.30 after</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2">
         <v>12.3</v>
@@ -1268,10 +1257,10 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="str">
         <f t="shared" si="2"/>
-        <v>¥12.30 after</v>
+        <v>before ¥12.30</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2">
         <v>12.3</v>
@@ -1282,14 +1271,14 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>before ¥12.30</v>
+        <f t="shared" si="0"/>
+        <v>-a $12.30 profit</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" s="2">
-        <v>12.3</v>
+        <v>-12.3</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>66</v>
@@ -1298,10 +1287,10 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-a $12.30 profit</v>
+        <v>-¥12.30 after</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="2">
         <v>-12.3</v>
@@ -1313,10 +1302,10 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-¥12.30 after</v>
+        <v>-before ¥12.30</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2">
         <v>-12.3</v>
@@ -1325,28 +1314,28 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-before ¥12.30</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="2">
-        <v>-12.3</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>66</v>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="9" t="str">
+        <f t="shared" ref="A24:A39" si="3">TEXT(C24, B24)</f>
+        <v>1,234,567</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1234567</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="str">
-        <f t="shared" ref="A25:A40" si="3">TEXT(C25, B25)</f>
+        <f t="shared" si="3"/>
         <v>1,234,567</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C25" s="2">
         <v>1234567</v>
@@ -1361,7 +1350,7 @@
         <v>1,234,567</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C26" s="2">
         <v>1234567</v>
@@ -1373,10 +1362,10 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>1,234,567</v>
+        <v>,1234567</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C27" s="2">
         <v>1234567</v>
@@ -1388,10 +1377,10 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>,1234567</v>
+        <v>1,234,567.</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2">
         <v>1234567</v>
@@ -1403,10 +1392,10 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>1,234,567.</v>
+        <v>1,234,567</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2">
         <v>1234567</v>
@@ -1421,7 +1410,7 @@
         <v>1,234,567</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2">
         <v>1234567</v>
@@ -1436,7 +1425,7 @@
         <v>1,234,567</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C31" s="2">
         <v>1234567</v>
@@ -1448,10 +1437,10 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>1,234,567</v>
+        <v>,1234567</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C32" s="2">
         <v>1234567</v>
@@ -1463,10 +1452,10 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>,1234567</v>
+        <v>1,234,567.0</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C33" s="2">
         <v>1234567</v>
@@ -1478,13 +1467,13 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>1,234,567.0</v>
+        <v>12</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C34" s="2">
-        <v>1234567</v>
+        <v>12</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>67</v>
@@ -1493,13 +1482,13 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C35" s="2">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>67</v>
@@ -1508,13 +1497,13 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>123</v>
+        <v>1,234</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C36" s="2">
-        <v>123</v>
+        <v>1234</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>67</v>
@@ -1523,13 +1512,13 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>1,234</v>
+        <v>12,345</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C37" s="2">
-        <v>1234</v>
+        <v>12345</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>67</v>
@@ -1538,13 +1527,13 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>12,345</v>
+        <v>123,456</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C38" s="2">
-        <v>12345</v>
+        <v>123456</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>67</v>
@@ -1553,13 +1542,13 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>123,456</v>
+        <v>1,234,567</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C39" s="2">
-        <v>123456</v>
+        <v>1234567</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>67</v>
@@ -1567,11 +1556,11 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A40:A46" si="4">TEXT(C40, B40)</f>
         <v>1,234,567</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="C40" s="2">
         <v>1234567</v>
@@ -1582,11 +1571,11 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="str">
-        <f t="shared" ref="A41:A47" si="4">TEXT(C41, B41)</f>
+        <f t="shared" si="4"/>
         <v>1,234,567</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C41" s="2">
         <v>1234567</v>
@@ -1601,7 +1590,7 @@
         <v>1,234,567</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C42" s="2">
         <v>1234567</v>
@@ -1616,7 +1605,7 @@
         <v>1,234,567</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C43" s="2">
         <v>1234567</v>
@@ -1628,10 +1617,10 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="str">
         <f t="shared" si="4"/>
-        <v>1,234,567</v>
+        <v xml:space="preserve"> 1,234,567</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C44" s="2">
         <v>1234567</v>
@@ -1643,10 +1632,10 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve"> 1,234,567</v>
+        <v xml:space="preserve">  1,234,567</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C45" s="2">
         <v>1234567</v>
@@ -1658,10 +1647,10 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">  1,234,567</v>
+        <v xml:space="preserve">    1,234,567</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="C46" s="2">
         <v>1234567</v>
@@ -1672,14 +1661,14 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">    1,234,567</v>
+        <f t="shared" ref="A47:A52" si="5">TEXT(C47, B47)</f>
+        <v>12</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="C47" s="2">
-        <v>1234567</v>
+        <v>12</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>67</v>
@@ -1687,14 +1676,14 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="9" t="str">
-        <f t="shared" ref="A48:A53" si="5">TEXT(C48, B48)</f>
-        <v>12</v>
+        <f t="shared" si="5"/>
+        <v>123</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C48" s="2">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>67</v>
@@ -1703,13 +1692,13 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>123</v>
+        <v>1,234</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C49" s="2">
-        <v>123</v>
+        <v>1234</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>67</v>
@@ -1718,13 +1707,13 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>1,234</v>
+        <v>12,345</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C50" s="2">
-        <v>1234</v>
+        <v>12345</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>67</v>
@@ -1733,13 +1722,13 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>12,345</v>
+        <v>123,456</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C51" s="2">
-        <v>12345</v>
+        <v>123456</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>67</v>
@@ -1748,13 +1737,13 @@
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>123,456</v>
+        <v>1,234,567</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C52" s="2">
-        <v>123456</v>
+        <v>1234567</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>67</v>
@@ -1762,14 +1751,14 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="9" t="str">
-        <f t="shared" si="5"/>
-        <v>1,234,567</v>
+        <f t="shared" si="0"/>
+        <v>-1,234,567</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>114</v>
+        <v>42</v>
       </c>
       <c r="C53" s="2">
-        <v>1234567</v>
+        <v>-1234567</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>67</v>
@@ -1781,7 +1770,7 @@
         <v>-1,234,567</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C54" s="2">
         <v>-1234567</v>
@@ -1796,7 +1785,7 @@
         <v>-1,234,567</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C55" s="2">
         <v>-1234567</v>
@@ -1808,10 +1797,10 @@
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-1,234,567</v>
+        <v>-,1234567</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C56" s="2">
         <v>-1234567</v>
@@ -1823,10 +1812,10 @@
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-,1234567</v>
+        <v>-1,234,567.</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C57" s="2">
         <v>-1234567</v>
@@ -1838,10 +1827,10 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-1,234,567.</v>
+        <v>-1,234,567</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C58" s="2">
         <v>-1234567</v>
@@ -1856,7 +1845,7 @@
         <v>-1,234,567</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C59" s="2">
         <v>-1234567</v>
@@ -1871,7 +1860,7 @@
         <v>-1,234,567</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C60" s="2">
         <v>-1234567</v>
@@ -1883,10 +1872,10 @@
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-1,234,567</v>
+        <v>-,1234567</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C61" s="2">
         <v>-1234567</v>
@@ -1898,10 +1887,10 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-,1234567</v>
+        <v>-1,234,567.0</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C62" s="2">
         <v>-1234567</v>
@@ -1912,14 +1901,14 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-1,234,567.0</v>
+        <f t="shared" ref="A63:A69" si="6">TEXT(C63, B63)</f>
+        <v>1,234,567</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C63" s="2">
-        <v>-1234567</v>
+        <v>1234567</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>67</v>
@@ -1927,11 +1916,11 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="9" t="str">
-        <f t="shared" ref="A64:A70" si="6">TEXT(C64, B64)</f>
+        <f t="shared" si="6"/>
         <v>1,234,567</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C64" s="2">
         <v>1234567</v>
@@ -1946,7 +1935,7 @@
         <v>1,234,567</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C65" s="2">
         <v>1234567</v>
@@ -1961,7 +1950,7 @@
         <v>1,234,567</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C66" s="2">
         <v>1234567</v>
@@ -1973,10 +1962,10 @@
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>1,234,567</v>
+        <v>01,234,567</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C67" s="2">
         <v>1234567</v>
@@ -1988,10 +1977,10 @@
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>01,234,567</v>
+        <v>001,234,567</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C68" s="2">
         <v>1234567</v>
@@ -2003,10 +1992,10 @@
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>001,234,567</v>
+        <v>0,001,234,567</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="C69" s="2">
         <v>1234567</v>
@@ -2017,14 +2006,14 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>0,001,234,567</v>
+        <f t="shared" ref="A70:A75" si="7">TEXT(C70, B70)</f>
+        <v>-12</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="C70" s="2">
-        <v>1234567</v>
+        <v>-12</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>67</v>
@@ -2032,14 +2021,14 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A71" s="9" t="str">
-        <f t="shared" ref="A71:A76" si="7">TEXT(C71, B71)</f>
-        <v>-12</v>
+        <f t="shared" si="7"/>
+        <v>-123</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C71" s="2">
-        <v>-12</v>
+        <v>-123</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>67</v>
@@ -2048,13 +2037,13 @@
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>-123</v>
+        <v>-1,234</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C72" s="2">
-        <v>-123</v>
+        <v>-1234</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>67</v>
@@ -2063,13 +2052,13 @@
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A73" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>-1,234</v>
+        <v>-12,345</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C73" s="2">
-        <v>-1234</v>
+        <v>-12345</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>67</v>
@@ -2078,13 +2067,13 @@
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A74" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>-12,345</v>
+        <v>-123,456</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C74" s="2">
-        <v>-12345</v>
+        <v>-123456</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>67</v>
@@ -2093,13 +2082,13 @@
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>-123,456</v>
+        <v>-1,234,567</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C75" s="2">
-        <v>-123456</v>
+        <v>-1234567</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>67</v>
@@ -2107,11 +2096,11 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A76:A82" si="8">TEXT(C76, B76)</f>
         <v>-1,234,567</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="C76" s="2">
         <v>-1234567</v>
@@ -2122,11 +2111,11 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" s="9" t="str">
-        <f t="shared" ref="A77:A83" si="8">TEXT(C77, B77)</f>
+        <f t="shared" si="8"/>
         <v>-1,234,567</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C77" s="2">
         <v>-1234567</v>
@@ -2141,7 +2130,7 @@
         <v>-1,234,567</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C78" s="2">
         <v>-1234567</v>
@@ -2156,7 +2145,7 @@
         <v>-1,234,567</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C79" s="2">
         <v>-1234567</v>
@@ -2168,10 +2157,10 @@
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>-1,234,567</v>
+        <v>- 1,234,567</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C80" s="2">
         <v>-1234567</v>
@@ -2183,10 +2172,10 @@
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>- 1,234,567</v>
+        <v>-  1,234,567</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C81" s="2">
         <v>-1234567</v>
@@ -2198,10 +2187,10 @@
     <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>-  1,234,567</v>
+        <v>-    1,234,567</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="C82" s="2">
         <v>-1234567</v>
@@ -2212,14 +2201,14 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>-    1,234,567</v>
+        <f t="shared" ref="A83:A91" si="9">TEXT(C83, B83)</f>
+        <v>-12</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="C83" s="2">
-        <v>-1234567</v>
+        <v>-12</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>67</v>
@@ -2227,14 +2216,14 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" s="9" t="str">
-        <f t="shared" ref="A84:A92" si="9">TEXT(C84, B84)</f>
-        <v>-12</v>
+        <f t="shared" si="9"/>
+        <v>-123</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C84" s="2">
-        <v>-12</v>
+        <v>-123</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>67</v>
@@ -2243,13 +2232,13 @@
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>-123</v>
+        <v>-1,234</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C85" s="2">
-        <v>-123</v>
+        <v>-1234</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>67</v>
@@ -2258,13 +2247,13 @@
     <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>-1,234</v>
+        <v>-12,345</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C86" s="2">
-        <v>-1234</v>
+        <v>-12345</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>67</v>
@@ -2273,13 +2262,13 @@
     <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>-12,345</v>
+        <v>-123,456</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C87" s="2">
-        <v>-12345</v>
+        <v>-123456</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>67</v>
@@ -2288,40 +2277,40 @@
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>-123,456</v>
+        <v>-1,234,567</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C88" s="2">
-        <v>-123456</v>
+        <v>-1234567</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A89" s="9" t="str">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A90" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>-1,234,567</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C89" s="2">
-        <v>-1234567</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>67</v>
+        <v>1235</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C90" s="2">
+        <v>1234567</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>1235</v>
+        <v>1</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C91" s="2">
         <v>1234567</v>
@@ -2332,11 +2321,11 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" s="9" t="str">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <f t="shared" ref="A92:A93" si="10">TEXT(C92, B92)</f>
+        <v>1234.6</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C92" s="2">
         <v>1234567</v>
@@ -2347,11 +2336,11 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" s="9" t="str">
-        <f t="shared" ref="A93:A94" si="10">TEXT(C93, B93)</f>
-        <v>1234.6</v>
+        <f t="shared" si="10"/>
+        <v>1.2</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C93" s="2">
         <v>1234567</v>
@@ -2362,14 +2351,14 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" s="9" t="str">
-        <f t="shared" si="10"/>
-        <v>1.2</v>
+        <f t="shared" si="0"/>
+        <v>-1235</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C94" s="2">
-        <v>1234567</v>
+        <v>-1234567</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>68</v>
@@ -2378,10 +2367,10 @@
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-1235</v>
+        <v>-1</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C95" s="2">
         <v>-1234567</v>
@@ -2393,10 +2382,10 @@
     <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-1234.6</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C96" s="2">
         <v>-1234567</v>
@@ -2408,10 +2397,10 @@
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>-1234.6</v>
+        <v>-1.2</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C97" s="2">
         <v>-1234567</v>
@@ -2421,30 +2410,35 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A98" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-1.2</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C98" s="2">
-        <v>-1234567</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>68</v>
+      <c r="A98" s="11"/>
+      <c r="B98" s="11"/>
+      <c r="D98" s="7"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A99" s="9" t="str">
+        <f t="shared" ref="A99:A101" si="11">TEXT(C99, B99)</f>
+        <v>1.23%</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C99" s="2">
+        <v>1.23E-2</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" s="9" t="str">
-        <f t="shared" ref="A100:A102" si="11">TEXT(C100, B100)</f>
-        <v>1.23%</v>
+        <f t="shared" si="11"/>
+        <v>12,345.00%</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C100" s="2">
-        <v>1.23E-2</v>
+        <v>123.45</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>69</v>
@@ -2453,10 +2447,10 @@
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" s="9" t="str">
         <f t="shared" si="11"/>
-        <v>12,345.00%</v>
+        <v>1,234,500.00%%</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="C101" s="2">
         <v>123.45</v>
@@ -2467,14 +2461,14 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" s="9" t="str">
-        <f t="shared" si="11"/>
-        <v>1,234,500.00%%</v>
+        <f>TEXT(C102, B102)</f>
+        <v>-1.23%</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="C102" s="2">
-        <v>123.45</v>
+        <v>-1.23E-2</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>69</v>
@@ -2482,14 +2476,14 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-1.23%</v>
+        <f>TEXT(C103, B103)</f>
+        <v>-12,345.00%</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C103" s="2">
-        <v>-1.23E-2</v>
+        <v>-123.45</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>69</v>
@@ -2497,11 +2491,11 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-12,345.00%</v>
+        <f>TEXT(C104, B104)</f>
+        <v>-1,234,500.00%%</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="C104" s="2">
         <v>-123.45</v>
@@ -2512,21 +2506,18 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>-1,234,500.00%%</v>
-      </c>
-      <c r="B105" s="9" t="s">
-        <v>64</v>
+        <f>TEXT(C105, B105)</f>
+        <v>0.04%</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="C105" s="2">
-        <v>-123.45</v>
+        <v>3.5E-4</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="D106" s="7"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A107" s="9" t="str">
@@ -3805,7 +3796,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A194" s="9" t="str">
-        <f t="shared" ref="A194:A197" si="30">TEXT(C194, B194)</f>
+        <f t="shared" ref="A194:A196" si="30">TEXT(C194, B194)</f>
         <v>|0 =/=1|</v>
       </c>
       <c r="B194" s="9" t="s">
@@ -5668,7 +5659,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A319" s="9" t="str">
-        <f t="shared" ref="A319:A336" si="36">TEXT(C319, B319)</f>
+        <f t="shared" ref="A319:A332" si="36">TEXT(C319, B319)</f>
         <v>-|1      |</v>
       </c>
       <c r="B319" s="9" t="s">

</xml_diff>